<commit_message>
BalaRaju - Working on Payslip pdf module
</commit_message>
<xml_diff>
--- a/public/PAYSLIPS/October-2014-bank_statement.xlsx
+++ b/public/PAYSLIPS/October-2014-bank_statement.xlsx
@@ -75,7 +75,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.38988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
@@ -125,7 +125,7 @@
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>870146000000.0</v>
+        <v>8701.46</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>

</xml_diff>